<commit_message>
trying and failing to parallelize
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\Python_Scripts\Plane_ticket_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2713D-A6A2-42D6-A9C2-810EB72BF7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCC2BD-7498-4EBF-AE93-2B538422C2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13215" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1272" yWindow="1056" windowWidth="17304" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3">
-        <v>44751.940891203703</v>
+        <v>44752.590358796297</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -530,6 +530,9 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E8">
+        <v>240</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -545,6 +548,9 @@
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E9">
+        <v>228</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -560,6 +566,9 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E10">
+        <v>256</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -575,6 +584,9 @@
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E11">
+        <v>471</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -590,6 +602,9 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E12">
+        <v>467</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -605,6 +620,9 @@
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E13">
+        <v>396</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -620,6 +638,9 @@
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E14">
+        <v>281</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -635,6 +656,9 @@
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E15">
+        <v>459</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -650,8 +674,11 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>44824</v>
@@ -665,8 +692,11 @@
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>44830</v>
@@ -680,8 +710,11 @@
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>44831</v>
@@ -695,8 +728,11 @@
       <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>44837</v>
@@ -710,8 +746,11 @@
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>44838</v>
@@ -725,8 +764,11 @@
       <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>44844</v>
@@ -740,8 +782,11 @@
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>44845</v>
@@ -755,8 +800,11 @@
       <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>44851</v>
@@ -770,8 +818,11 @@
       <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>44852</v>
@@ -785,8 +836,11 @@
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>44858</v>
@@ -800,8 +854,11 @@
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>44859</v>
@@ -815,8 +872,11 @@
       <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>44865</v>
@@ -830,8 +890,11 @@
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>44866</v>
@@ -845,8 +908,11 @@
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>44872</v>
@@ -860,8 +926,11 @@
       <c r="D30" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>44873</v>
@@ -875,8 +944,11 @@
       <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>44879</v>
@@ -890,8 +962,11 @@
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>44880</v>
@@ -905,8 +980,11 @@
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>44886</v>
@@ -920,8 +998,11 @@
       <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>44887</v>
@@ -935,8 +1016,11 @@
       <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>44893</v>
@@ -950,8 +1034,11 @@
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>44894</v>
@@ -965,8 +1052,11 @@
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>44900</v>
@@ -980,8 +1070,11 @@
       <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>44901</v>
@@ -995,8 +1088,11 @@
       <c r="D39" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>44907</v>
@@ -1010,8 +1106,11 @@
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>44908</v>
@@ -1025,8 +1124,11 @@
       <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>44914</v>
@@ -1040,8 +1142,11 @@
       <c r="D42" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>44915</v>
@@ -1055,8 +1160,11 @@
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>44921</v>
@@ -1070,8 +1178,11 @@
       <c r="D44" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>44922</v>
@@ -1085,8 +1196,11 @@
       <c r="D45" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>44928</v>
@@ -1100,8 +1214,11 @@
       <c r="D46" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>44929</v>
@@ -1115,8 +1232,11 @@
       <c r="D47" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>44935</v>
@@ -1130,8 +1250,11 @@
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>44936</v>
@@ -1145,8 +1268,11 @@
       <c r="D49" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>44942</v>
@@ -1161,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>44943</v>
@@ -1176,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>44949</v>
@@ -1191,7 +1317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>44950</v>
@@ -1206,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>44956</v>
@@ -1221,7 +1347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>44957</v>
@@ -1236,7 +1362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>44963</v>
@@ -1251,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>44964</v>
@@ -1266,7 +1392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>44970</v>
@@ -1281,7 +1407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>44971</v>
@@ -1296,7 +1422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>44977</v>
@@ -1311,7 +1437,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>44978</v>
@@ -1326,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <f t="shared" si="0"/>
         <v>44984</v>
@@ -1341,7 +1467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f t="shared" si="0"/>
         <v>44985</v>
@@ -1356,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f t="shared" si="0"/>
         <v>44991</v>

</xml_diff>